<commit_message>
TDMS data loading is implemented and working well. Additionally, now TDMS open times are much better, size of the saved file is greatly reduced. Bridge swap function has been fixed. Incorrect TTL status saving has been fixed. "Loading" progress bar functions much better now.
</commit_message>
<xml_diff>
--- a/Data_loading_speed.xlsx
+++ b/Data_loading_speed.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26592" windowHeight="9504"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26592" windowHeight="9504" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CSV" sheetId="1" r:id="rId1"/>
+    <sheet name="TDMS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,20 +25,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Time to load, ms</t>
   </si>
   <si>
     <t>Record length, s</t>
+  </si>
+  <si>
+    <t>Record length, samples</t>
+  </si>
+  <si>
+    <t>Time top load data only, ms</t>
+  </si>
+  <si>
+    <t>Time to load whole file (incl. opening), ms</t>
+  </si>
+  <si>
+    <t>Time to open only, ms</t>
+  </si>
+  <si>
+    <t>Index present</t>
+  </si>
+  <si>
+    <t>Index re-creation</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>On</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Data loading rate</t>
+  </si>
+  <si>
+    <t>Full set loading rate</t>
+  </si>
+  <si>
+    <t>File size, KB</t>
+  </si>
+  <si>
+    <t>Index size, KB</t>
+  </si>
+  <si>
+    <t>Total size, KB</t>
+  </si>
+  <si>
+    <t>Rate, KB/s</t>
+  </si>
+  <si>
+    <t>Fully defragmented, chunk size 1</t>
+  </si>
+  <si>
+    <t>Raw, no defragmentation, chunk size 1</t>
+  </si>
+  <si>
+    <t>Raw, no defragmentation, chunk size 400</t>
+  </si>
+  <si>
+    <t>Fully defragmented, chunk size 400</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -65,8 +145,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,7 +233,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>CSV!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -224,7 +317,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>CSV!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -245,7 +338,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:f>CSV!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -274,11 +367,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="581830464"/>
-        <c:axId val="581831640"/>
+        <c:axId val="560781208"/>
+        <c:axId val="560780816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="581830464"/>
+        <c:axId val="560781208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -391,12 +484,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="581831640"/>
+        <c:crossAx val="560780816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="581831640"/>
+        <c:axId val="560780816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,7 +602,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="581830464"/>
+        <c:crossAx val="560781208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1118,16 +1211,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1412,60 +1505,595 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>30</v>
       </c>
       <c r="B2">
         <v>40</v>
       </c>
+      <c r="C2">
+        <f>A2/(B2/1000)</f>
+        <v>750</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>100</v>
       </c>
       <c r="B3">
         <v>130</v>
       </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C5" si="0">A3/(B3/1000)</f>
+        <v>769.23076923076917</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>200</v>
       </c>
       <c r="B4">
         <v>253</v>
       </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>790.51383399209487</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>360</v>
       </c>
       <c r="B5">
         <v>470</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>765.95744680851067</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>100000</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>1229.73</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>215113</v>
+      </c>
+      <c r="G2" s="5">
+        <f>F2-H2</f>
+        <v>181485</v>
+      </c>
+      <c r="H2">
+        <v>33628</v>
+      </c>
+      <c r="I2" s="5">
+        <f>D2/(H2/1000)</f>
+        <v>36.568633281788983</v>
+      </c>
+      <c r="J2" s="5">
+        <f>D2/(F2/1000)</f>
+        <v>5.7166698432916654</v>
+      </c>
+      <c r="K2" s="7">
+        <v>4202699</v>
+      </c>
+      <c r="L2" s="7">
+        <v>3202208</v>
+      </c>
+      <c r="M2" s="7">
+        <f>K2+L2</f>
+        <v>7404907</v>
+      </c>
+      <c r="N2">
+        <f>M2/53231.3</f>
+        <v>139.10813750556534</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>100000</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>1229.73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>210282</v>
+      </c>
+      <c r="G3" s="5">
+        <f>F3-H3</f>
+        <v>177732</v>
+      </c>
+      <c r="H3">
+        <v>32550</v>
+      </c>
+      <c r="I3" s="5">
+        <f>D3/(H3/1000)</f>
+        <v>37.779723502304151</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" ref="J3:J9" si="0">D3/(F3/1000)</f>
+        <v>5.8480041087682251</v>
+      </c>
+      <c r="K3" s="7">
+        <v>4202699</v>
+      </c>
+      <c r="L3" s="7">
+        <v>3202208</v>
+      </c>
+      <c r="M3" s="7">
+        <f t="shared" ref="M3:M9" si="1">K3+L3</f>
+        <v>7404907</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N10" si="2">M3/53231.3</f>
+        <v>139.10813750556534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>100000</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1229.73</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>919365</v>
+      </c>
+      <c r="G4" s="5">
+        <f>F4-H4</f>
+        <v>886769</v>
+      </c>
+      <c r="H4">
+        <v>32596</v>
+      </c>
+      <c r="I4" s="5">
+        <f>D4/(H4/1000)</f>
+        <v>37.726408148239052</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" si="0"/>
+        <v>1.3375862687833451</v>
+      </c>
+      <c r="K4" s="7">
+        <v>4202699</v>
+      </c>
+      <c r="L4" s="7">
+        <v>3202208</v>
+      </c>
+      <c r="M4" s="7">
+        <f t="shared" si="1"/>
+        <v>7404907</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>139.10813750556534</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>100000</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>1229.73</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>209443</v>
+      </c>
+      <c r="G5" s="5">
+        <f>F5-H5</f>
+        <v>176948</v>
+      </c>
+      <c r="H5">
+        <v>32495</v>
+      </c>
+      <c r="I5" s="5">
+        <f>D5/(H5/1000)</f>
+        <v>37.843668256654873</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" si="0"/>
+        <v>5.8714304130479409</v>
+      </c>
+      <c r="K5" s="7">
+        <v>4202699</v>
+      </c>
+      <c r="L5" s="7">
+        <v>3202208</v>
+      </c>
+      <c r="M5" s="7">
+        <f t="shared" si="1"/>
+        <v>7404907</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>139.10813750556534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>100000</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>1229.73</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6">
+        <v>2555</v>
+      </c>
+      <c r="G6" s="5">
+        <f>F6-H6</f>
+        <v>113</v>
+      </c>
+      <c r="H6">
+        <v>2442</v>
+      </c>
+      <c r="I6" s="5">
+        <f>D6/(H6/1000)</f>
+        <v>503.57493857493853</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="0"/>
+        <v>481.30332681017609</v>
+      </c>
+      <c r="K6" s="7">
+        <v>1000493</v>
+      </c>
+      <c r="L6" s="7">
+        <v>3</v>
+      </c>
+      <c r="M6" s="7">
+        <f t="shared" si="1"/>
+        <v>1000496</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>18.795257677343969</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>500000</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>6152.12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>12406</v>
+      </c>
+      <c r="G7" s="5">
+        <f>F7-H7</f>
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>12386</v>
+      </c>
+      <c r="I7" s="5">
+        <f>D7/(H7/1000)</f>
+        <v>496.69949943484579</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="0"/>
+        <v>495.89875866516201</v>
+      </c>
+      <c r="K7" s="7">
+        <v>1000493</v>
+      </c>
+      <c r="L7" s="7">
+        <v>3</v>
+      </c>
+      <c r="M7" s="7">
+        <f t="shared" si="1"/>
+        <v>1000496</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>18.795257677343969</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4331338</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>53231.3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8">
+        <v>107766</v>
+      </c>
+      <c r="G8" s="5">
+        <f>F8-H8</f>
+        <v>19</v>
+      </c>
+      <c r="H8">
+        <v>107747</v>
+      </c>
+      <c r="I8" s="5">
+        <f>D8/(H8/1000)</f>
+        <v>494.03974124569595</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="0"/>
+        <v>493.95263812334133</v>
+      </c>
+      <c r="K8" s="7">
+        <v>1000493</v>
+      </c>
+      <c r="L8" s="7">
+        <v>3</v>
+      </c>
+      <c r="M8" s="7">
+        <f t="shared" si="1"/>
+        <v>1000496</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>18.795257677343969</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>11373</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>143.60300000000001</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9">
+        <v>313</v>
+      </c>
+      <c r="G9" s="5">
+        <f>F9-H9</f>
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>308</v>
+      </c>
+      <c r="I9" s="5">
+        <f>D9/(H9/1000)</f>
+        <v>466.24350649350652</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="0"/>
+        <v>458.79552715654955</v>
+      </c>
+      <c r="K9" s="7">
+        <v>2618</v>
+      </c>
+      <c r="L9" s="7">
+        <v>24</v>
+      </c>
+      <c r="M9" s="7">
+        <f t="shared" si="1"/>
+        <v>2642</v>
+      </c>
+      <c r="N9">
+        <f>M9/143.603</f>
+        <v>18.397944332639288</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>11373</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>143.60300000000001</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10">
+        <v>303</v>
+      </c>
+      <c r="G10" s="5">
+        <f>F10-H10</f>
+        <v>22</v>
+      </c>
+      <c r="H10">
+        <v>281</v>
+      </c>
+      <c r="I10" s="5">
+        <f>D10/(H10/1000)</f>
+        <v>511.04270462633451</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" ref="J10" si="3">D10/(F10/1000)</f>
+        <v>473.93729372937298</v>
+      </c>
+      <c r="K10" s="7">
+        <v>2597</v>
+      </c>
+      <c r="L10" s="7">
+        <v>3</v>
+      </c>
+      <c r="M10" s="7">
+        <f t="shared" ref="M10" si="4">K10+L10</f>
+        <v>2600</v>
+      </c>
+      <c r="N10">
+        <f>M10/143.603</f>
+        <v>18.105471334164328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>